<commit_message>
cập nhật theo yêu cầu của Hoàng Trần
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0013 Cap nhat phieu chuyen kho.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/WF0013 Cap nhat phieu chuyen kho.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ASOFT_ERP8.1\10_DOCUMENT\13_DETAIL_DESIGN\2.PROJECTS\2015\0.ERP PROJECTS\2.Quan ly mat hang theo quy cach\ASOFT-WM\2015-06-19 Phieu van chuyen noi bo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SOFT\201512\10_DOCUMENT\13_DETAIL_DESIGN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="1" r:id="rId1"/>
@@ -1952,7 +1952,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="269">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2911,6 +2911,86 @@
 UnitPrice04, UnitPrice05, UnitPrice06, UnitPrice07, UnitPrice08, UnitPrice09, UnitPrice10, UnitPrice11,
 UnitPrice12, UnitPrice13, UnitPrice14, UnitPrice15, UnitPrice16, UnitPrice17, UnitPrice18, UnitPrice19, UnitPrice20, UnitPriceStandard)
 VALUES @</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thị Phượng </t>
+  </si>
+  <si>
+    <t>Thị Phượng</t>
+  </si>
+  <si>
+    <t>Sửa</t>
+  </si>
+  <si>
+    <t>Require</t>
+  </si>
+  <si>
+    <t>Click LinkEdit</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>WFML000185</t>
+  </si>
+  <si>
+    <t>AT2006</t>
+  </si>
+  <si>
+    <t>ID SQL</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT TOP 1 1 FROM AT2006
+WHERE DivisionID = @DivisionID
+AND VoucherID = @VoucherID </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>AND IsWeb=1</t>
+    </r>
+  </si>
+  <si>
+    <t>@DivisionID @VoucherID
+@IsWeb</t>
+  </si>
+  <si>
+    <t>@@DivisionID
+@@VoucherID
+1</t>
+  </si>
+  <si>
+    <t>LinkEdit</t>
+  </si>
+  <si>
+    <t>Kiểm tra điều kiện IsWeb khi thực hiện Sửa phiếu cập nhật</t>
+  </si>
+  <si>
+    <t>@SQL005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chỉ dùng cho Customize Hoàng Trần (CustomizeIndex = 51) Thực hiện câu @SQL005 để kiểm tra điệu kiện để load màn hình Cập nhật khi thực hiện Click LinkEdit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver 3.0 </t>
+  </si>
+  <si>
+    <t>CustomizeIndex =51
+Click LickEdit Thực thi @SQL0005 để kiểm tra điều kiện IsWeb,
+- Nếu =1 cảnh báo message WFML000185, nếu Click OK thực thi câu @SQL004 để load Form WF0013 nhưng Disabled tất cả các trường, nếu Click No thực hiện thoát
+- Nếu =0 thực hiện @SQL004 để load form WF0013</t>
+  </si>
+  <si>
+    <t>- CustomizeIndex = 51 (Hoàng Trần ) Kiểm tra điều kiện trước khi sửa
++ sheet Input check Thêm WFML000185 
++ sheet Data Input thêm @SQL005
++ Sheet Form Func Spec Thêm xử lý khi sửa</t>
   </si>
 </sst>
 </file>
@@ -3366,7 +3446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="282">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3888,6 +3968,63 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3918,71 +4055,29 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4002,24 +4097,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4100,6 +4177,63 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4109,13 +4243,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FF990000"/>
       <color rgb="FF008080"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FF66FFFF"/>
     </mruColors>
   </colors>
@@ -4438,8 +4572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:J13"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4458,10 +4592,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -4483,11 +4617,13 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126"/>
+      <c r="J1" s="126" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -4509,7 +4645,9 @@
       <c r="I2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="15">
+        <v>42381</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
@@ -4536,14 +4674,14 @@
       <c r="D4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="216" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="197"/>
-      <c r="G4" s="197"/>
-      <c r="H4" s="197"/>
-      <c r="I4" s="197"/>
-      <c r="J4" s="197"/>
+      <c r="F4" s="216"/>
+      <c r="G4" s="216"/>
+      <c r="H4" s="216"/>
+      <c r="I4" s="216"/>
+      <c r="J4" s="216"/>
     </row>
     <row r="5" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -4560,14 +4698,14 @@
         <f>H1</f>
         <v>Thanh Sơn</v>
       </c>
-      <c r="E5" s="198" t="s">
+      <c r="E5" s="217" t="s">
         <v>172</v>
       </c>
-      <c r="F5" s="199"/>
-      <c r="G5" s="199"/>
-      <c r="H5" s="199"/>
-      <c r="I5" s="199"/>
-      <c r="J5" s="199"/>
+      <c r="F5" s="218"/>
+      <c r="G5" s="218"/>
+      <c r="H5" s="218"/>
+      <c r="I5" s="218"/>
+      <c r="J5" s="218"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -4582,30 +4720,36 @@
       <c r="D6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="200" t="s">
+      <c r="E6" s="219" t="s">
         <v>240</v>
       </c>
-      <c r="F6" s="201"/>
-      <c r="G6" s="201"/>
-      <c r="H6" s="201"/>
-      <c r="I6" s="201"/>
-      <c r="J6" s="202"/>
-    </row>
-    <row r="7" spans="1:10" s="111" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="220"/>
+      <c r="G6" s="220"/>
+      <c r="H6" s="220"/>
+      <c r="I6" s="220"/>
+      <c r="J6" s="221"/>
+    </row>
+    <row r="7" spans="1:10" s="111" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112">
         <v>3</v>
       </c>
       <c r="B7" s="113">
         <v>3</v>
       </c>
-      <c r="C7" s="114"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="203"/>
-      <c r="F7" s="204"/>
-      <c r="G7" s="204"/>
-      <c r="H7" s="204"/>
-      <c r="I7" s="204"/>
-      <c r="J7" s="205"/>
+      <c r="C7" s="114">
+        <v>42381</v>
+      </c>
+      <c r="D7" s="115" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="263" t="s">
+        <v>268</v>
+      </c>
+      <c r="F7" s="222"/>
+      <c r="G7" s="222"/>
+      <c r="H7" s="222"/>
+      <c r="I7" s="222"/>
+      <c r="J7" s="223"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -4616,12 +4760,12 @@
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="193"/>
-      <c r="F8" s="194"/>
-      <c r="G8" s="194"/>
-      <c r="H8" s="194"/>
-      <c r="I8" s="194"/>
-      <c r="J8" s="195"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="213"/>
+      <c r="G8" s="213"/>
+      <c r="H8" s="213"/>
+      <c r="I8" s="213"/>
+      <c r="J8" s="214"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -4632,12 +4776,12 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="207"/>
-      <c r="F9" s="208"/>
-      <c r="G9" s="208"/>
-      <c r="H9" s="208"/>
-      <c r="I9" s="208"/>
-      <c r="J9" s="209"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="195"/>
+      <c r="G9" s="195"/>
+      <c r="H9" s="195"/>
+      <c r="I9" s="195"/>
+      <c r="J9" s="196"/>
     </row>
     <row r="10" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -4648,12 +4792,12 @@
       </c>
       <c r="C10" s="117"/>
       <c r="D10" s="118"/>
-      <c r="E10" s="210"/>
-      <c r="F10" s="211"/>
-      <c r="G10" s="211"/>
-      <c r="H10" s="211"/>
-      <c r="I10" s="211"/>
-      <c r="J10" s="212"/>
+      <c r="E10" s="197"/>
+      <c r="F10" s="198"/>
+      <c r="G10" s="198"/>
+      <c r="H10" s="198"/>
+      <c r="I10" s="198"/>
+      <c r="J10" s="199"/>
     </row>
     <row r="11" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -4664,12 +4808,12 @@
       </c>
       <c r="C11" s="120"/>
       <c r="D11" s="121"/>
-      <c r="E11" s="213"/>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="215"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="201"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="201"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="202"/>
     </row>
     <row r="12" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -4680,12 +4824,12 @@
       </c>
       <c r="C12" s="123"/>
       <c r="D12" s="124"/>
-      <c r="E12" s="216"/>
-      <c r="F12" s="217"/>
-      <c r="G12" s="217"/>
-      <c r="H12" s="217"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="218"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="204"/>
+      <c r="G12" s="204"/>
+      <c r="H12" s="204"/>
+      <c r="I12" s="204"/>
+      <c r="J12" s="205"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -4696,12 +4840,12 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="219"/>
-      <c r="F13" s="220"/>
-      <c r="G13" s="220"/>
-      <c r="H13" s="220"/>
-      <c r="I13" s="220"/>
-      <c r="J13" s="221"/>
+      <c r="E13" s="206"/>
+      <c r="F13" s="207"/>
+      <c r="G13" s="207"/>
+      <c r="H13" s="207"/>
+      <c r="I13" s="207"/>
+      <c r="J13" s="208"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -4712,361 +4856,369 @@
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="222"/>
-      <c r="F14" s="223"/>
-      <c r="G14" s="223"/>
-      <c r="H14" s="223"/>
-      <c r="I14" s="223"/>
-      <c r="J14" s="224"/>
+      <c r="E14" s="209"/>
+      <c r="F14" s="210"/>
+      <c r="G14" s="210"/>
+      <c r="H14" s="210"/>
+      <c r="I14" s="210"/>
+      <c r="J14" s="211"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="206"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="206"/>
-      <c r="F16" s="206"/>
-      <c r="G16" s="206"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="206"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="206"/>
-      <c r="F17" s="206"/>
-      <c r="G17" s="206"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="193"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="193"/>
+      <c r="J18" s="193"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="206"/>
-      <c r="F19" s="206"/>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="193"/>
+      <c r="G22" s="193"/>
+      <c r="H22" s="193"/>
+      <c r="I22" s="193"/>
+      <c r="J22" s="193"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="206"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
+      <c r="E23" s="193"/>
+      <c r="F23" s="193"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+      <c r="J23" s="193"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="206"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="193"/>
+      <c r="G24" s="193"/>
+      <c r="H24" s="193"/>
+      <c r="I24" s="193"/>
+      <c r="J24" s="193"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
+      <c r="E25" s="193"/>
+      <c r="F25" s="193"/>
+      <c r="G25" s="193"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="193"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="206"/>
-      <c r="F26" s="206"/>
-      <c r="G26" s="206"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="206"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="G26" s="193"/>
+      <c r="H26" s="193"/>
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="206"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="206"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="193"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="193"/>
+      <c r="J27" s="193"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="206"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="206"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="193"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="206"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="206"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="206"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="193"/>
+      <c r="G29" s="193"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="193"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="206"/>
-      <c r="F30" s="206"/>
-      <c r="G30" s="206"/>
-      <c r="H30" s="206"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="206"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="206"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="206"/>
-      <c r="F32" s="206"/>
-      <c r="G32" s="206"/>
-      <c r="H32" s="206"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="206"/>
+      <c r="E32" s="193"/>
+      <c r="F32" s="193"/>
+      <c r="G32" s="193"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="206"/>
-      <c r="F33" s="206"/>
-      <c r="G33" s="206"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="206"/>
+      <c r="E33" s="193"/>
+      <c r="F33" s="193"/>
+      <c r="G33" s="193"/>
+      <c r="H33" s="193"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="193"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="206"/>
-      <c r="F34" s="206"/>
-      <c r="G34" s="206"/>
-      <c r="H34" s="206"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="206"/>
+      <c r="E34" s="193"/>
+      <c r="F34" s="193"/>
+      <c r="G34" s="193"/>
+      <c r="H34" s="193"/>
+      <c r="I34" s="193"/>
+      <c r="J34" s="193"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="206"/>
-      <c r="F35" s="206"/>
-      <c r="G35" s="206"/>
-      <c r="H35" s="206"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="206"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="193"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="193"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="206"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="206"/>
-      <c r="F37" s="206"/>
-      <c r="G37" s="206"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="206"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="206"/>
-      <c r="F38" s="206"/>
-      <c r="G38" s="206"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="206"/>
+      <c r="E38" s="193"/>
+      <c r="F38" s="193"/>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="193"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="206"/>
-      <c r="F39" s="206"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="206"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="206"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="193"/>
+      <c r="H39" s="193"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="206"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="206"/>
-      <c r="F41" s="206"/>
-      <c r="G41" s="206"/>
-      <c r="H41" s="206"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="206"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="193"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="193"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="206"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="206"/>
-      <c r="H42" s="206"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="206"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="193"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
     <mergeCell ref="E32:J32"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
@@ -5079,24 +5231,16 @@
     <mergeCell ref="E29:J29"/>
     <mergeCell ref="E30:J30"/>
     <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E38:J38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -5305,10 +5449,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -5333,14 +5477,14 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -5367,7 +5511,7 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5383,72 +5527,72 @@
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="196" t="s">
+      <c r="A4" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="196"/>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
-      <c r="E4" s="196"/>
-      <c r="F4" s="196"/>
-      <c r="G4" s="196"/>
-      <c r="H4" s="196"/>
-      <c r="I4" s="196" t="s">
+      <c r="B4" s="215"/>
+      <c r="C4" s="215"/>
+      <c r="D4" s="215"/>
+      <c r="E4" s="215"/>
+      <c r="F4" s="215"/>
+      <c r="G4" s="215"/>
+      <c r="H4" s="215"/>
+      <c r="I4" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="196"/>
+      <c r="J4" s="215"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
-      <c r="C5" s="232"/>
-      <c r="D5" s="232"/>
-      <c r="E5" s="232"/>
-      <c r="F5" s="232"/>
-      <c r="G5" s="232"/>
-      <c r="H5" s="233"/>
-      <c r="I5" s="225" t="s">
+      <c r="A5" s="224"/>
+      <c r="B5" s="225"/>
+      <c r="C5" s="225"/>
+      <c r="D5" s="225"/>
+      <c r="E5" s="225"/>
+      <c r="F5" s="225"/>
+      <c r="G5" s="225"/>
+      <c r="H5" s="226"/>
+      <c r="I5" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="226"/>
+      <c r="J5" s="231"/>
     </row>
     <row r="6" spans="1:10" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="234"/>
-      <c r="B6" s="235"/>
-      <c r="C6" s="235"/>
-      <c r="D6" s="235"/>
-      <c r="E6" s="235"/>
-      <c r="F6" s="235"/>
-      <c r="G6" s="235"/>
-      <c r="H6" s="236"/>
-      <c r="I6" s="227" t="s">
+      <c r="A6" s="227"/>
+      <c r="B6" s="228"/>
+      <c r="C6" s="228"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="228"/>
+      <c r="H6" s="229"/>
+      <c r="I6" s="232" t="s">
         <v>248</v>
       </c>
-      <c r="J6" s="228"/>
+      <c r="J6" s="233"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="234"/>
-      <c r="B7" s="235"/>
-      <c r="C7" s="235"/>
-      <c r="D7" s="235"/>
-      <c r="E7" s="235"/>
-      <c r="F7" s="235"/>
-      <c r="G7" s="235"/>
-      <c r="H7" s="236"/>
-      <c r="I7" s="229" t="s">
+      <c r="A7" s="227"/>
+      <c r="B7" s="228"/>
+      <c r="C7" s="228"/>
+      <c r="D7" s="228"/>
+      <c r="E7" s="228"/>
+      <c r="F7" s="228"/>
+      <c r="G7" s="228"/>
+      <c r="H7" s="229"/>
+      <c r="I7" s="234" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="230"/>
+      <c r="J7" s="235"/>
     </row>
     <row r="8" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="234"/>
-      <c r="B8" s="235"/>
-      <c r="C8" s="235"/>
-      <c r="D8" s="235"/>
-      <c r="E8" s="235"/>
-      <c r="F8" s="235"/>
-      <c r="G8" s="235"/>
-      <c r="H8" s="236"/>
+      <c r="A8" s="227"/>
+      <c r="B8" s="228"/>
+      <c r="C8" s="228"/>
+      <c r="D8" s="228"/>
+      <c r="E8" s="228"/>
+      <c r="F8" s="228"/>
+      <c r="G8" s="228"/>
+      <c r="H8" s="229"/>
       <c r="I8" s="191" t="s">
         <v>241</v>
       </c>
@@ -5531,358 +5675,339 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="206"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="206"/>
-      <c r="F16" s="206"/>
-      <c r="G16" s="206"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="206"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="206"/>
-      <c r="F17" s="206"/>
-      <c r="G17" s="206"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="193"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="193"/>
+      <c r="J18" s="193"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="206"/>
-      <c r="F19" s="206"/>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="193"/>
+      <c r="G22" s="193"/>
+      <c r="H22" s="193"/>
+      <c r="I22" s="193"/>
+      <c r="J22" s="193"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="206"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
+      <c r="E23" s="193"/>
+      <c r="F23" s="193"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+      <c r="J23" s="193"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="206"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="193"/>
+      <c r="G24" s="193"/>
+      <c r="H24" s="193"/>
+      <c r="I24" s="193"/>
+      <c r="J24" s="193"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
+      <c r="E25" s="193"/>
+      <c r="F25" s="193"/>
+      <c r="G25" s="193"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="193"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="206"/>
-      <c r="F26" s="206"/>
-      <c r="G26" s="206"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="206"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="G26" s="193"/>
+      <c r="H26" s="193"/>
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="206"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="206"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="193"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="193"/>
+      <c r="J27" s="193"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="206"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="206"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="193"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="206"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="206"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="206"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="193"/>
+      <c r="G29" s="193"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="193"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="206"/>
-      <c r="F30" s="206"/>
-      <c r="G30" s="206"/>
-      <c r="H30" s="206"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="206"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="206"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="206"/>
-      <c r="F32" s="206"/>
-      <c r="G32" s="206"/>
-      <c r="H32" s="206"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="206"/>
+      <c r="E32" s="193"/>
+      <c r="F32" s="193"/>
+      <c r="G32" s="193"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="206"/>
-      <c r="F33" s="206"/>
-      <c r="G33" s="206"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="206"/>
+      <c r="E33" s="193"/>
+      <c r="F33" s="193"/>
+      <c r="G33" s="193"/>
+      <c r="H33" s="193"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="193"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="206"/>
-      <c r="F34" s="206"/>
-      <c r="G34" s="206"/>
-      <c r="H34" s="206"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="206"/>
+      <c r="E34" s="193"/>
+      <c r="F34" s="193"/>
+      <c r="G34" s="193"/>
+      <c r="H34" s="193"/>
+      <c r="I34" s="193"/>
+      <c r="J34" s="193"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="206"/>
-      <c r="F35" s="206"/>
-      <c r="G35" s="206"/>
-      <c r="H35" s="206"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="206"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="193"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="193"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="206"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="206"/>
-      <c r="F37" s="206"/>
-      <c r="G37" s="206"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="206"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="206"/>
-      <c r="F38" s="206"/>
-      <c r="G38" s="206"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="206"/>
+      <c r="E38" s="193"/>
+      <c r="F38" s="193"/>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="193"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="206"/>
-      <c r="F39" s="206"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="206"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="206"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="193"/>
+      <c r="H39" s="193"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="206"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="206"/>
-      <c r="F41" s="206"/>
-      <c r="G41" s="206"/>
-      <c r="H41" s="206"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="206"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="193"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="193"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="206"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="206"/>
-      <c r="H42" s="206"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="206"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="193"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A5:H8"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
     <mergeCell ref="E41:J41"/>
@@ -5899,6 +6024,25 @@
     <mergeCell ref="E37:J37"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A5:H8"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -5940,10 +6084,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="237"/>
+      <c r="B1" s="236"/>
       <c r="C1" s="128" t="s">
         <v>1</v>
       </c>
@@ -5968,18 +6112,18 @@
       <c r="I1" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="238">
+      <c r="J1" s="237" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
-      </c>
-      <c r="K1" s="239"/>
+        <v>Thị Phượng</v>
+      </c>
+      <c r="K1" s="238"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="237"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="236"/>
       <c r="C2" s="128" t="s">
         <v>7</v>
       </c>
@@ -6004,11 +6148,11 @@
       <c r="I2" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="240">
+      <c r="J2" s="239">
         <f>'Update History'!J2</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="241"/>
+        <v>42381</v>
+      </c>
+      <c r="K2" s="240"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -7721,7 +7865,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:J19"/>
+      <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7739,10 +7883,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -7767,14 +7911,14 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -7801,7 +7945,7 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -7838,23 +7982,33 @@
       <c r="G4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="245" t="s">
+      <c r="H4" s="244" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="245"/>
-      <c r="J4" s="245"/>
+      <c r="I4" s="244"/>
+      <c r="J4" s="244"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="242"/>
-      <c r="I5" s="243"/>
-      <c r="J5" s="244"/>
+      <c r="A5" s="264"/>
+      <c r="B5" s="265" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="266" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="267"/>
+      <c r="E5" s="268"/>
+      <c r="F5" s="269" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="269" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="270" t="s">
+        <v>256</v>
+      </c>
+      <c r="I5" s="271"/>
+      <c r="J5" s="272"/>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
@@ -7864,9 +8018,9 @@
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
-      <c r="H6" s="242"/>
-      <c r="I6" s="243"/>
-      <c r="J6" s="244"/>
+      <c r="H6" s="241"/>
+      <c r="I6" s="242"/>
+      <c r="J6" s="243"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="56"/>
@@ -7876,9 +8030,9 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-      <c r="H7" s="242"/>
-      <c r="I7" s="243"/>
-      <c r="J7" s="244"/>
+      <c r="H7" s="241"/>
+      <c r="I7" s="242"/>
+      <c r="J7" s="243"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
@@ -7888,9 +8042,9 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
-      <c r="H8" s="242"/>
-      <c r="I8" s="243"/>
-      <c r="J8" s="244"/>
+      <c r="H8" s="241"/>
+      <c r="I8" s="242"/>
+      <c r="J8" s="243"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -7900,9 +8054,9 @@
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="242"/>
-      <c r="I9" s="243"/>
-      <c r="J9" s="244"/>
+      <c r="H9" s="241"/>
+      <c r="I9" s="242"/>
+      <c r="J9" s="243"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
@@ -7912,9 +8066,9 @@
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="242"/>
-      <c r="I10" s="243"/>
-      <c r="J10" s="244"/>
+      <c r="H10" s="241"/>
+      <c r="I10" s="242"/>
+      <c r="J10" s="243"/>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
@@ -7924,9 +8078,9 @@
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="242"/>
-      <c r="I11" s="243"/>
-      <c r="J11" s="244"/>
+      <c r="H11" s="241"/>
+      <c r="I11" s="242"/>
+      <c r="J11" s="243"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
@@ -7936,9 +8090,9 @@
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
-      <c r="H12" s="242"/>
-      <c r="I12" s="243"/>
-      <c r="J12" s="244"/>
+      <c r="H12" s="241"/>
+      <c r="I12" s="242"/>
+      <c r="J12" s="243"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
@@ -7948,9 +8102,9 @@
       <c r="E13" s="55"/>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
-      <c r="H13" s="242"/>
-      <c r="I13" s="243"/>
-      <c r="J13" s="244"/>
+      <c r="H13" s="241"/>
+      <c r="I13" s="242"/>
+      <c r="J13" s="243"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="56"/>
@@ -7960,372 +8114,348 @@
       <c r="E14" s="55"/>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
-      <c r="H14" s="242"/>
-      <c r="I14" s="243"/>
-      <c r="J14" s="244"/>
+      <c r="H14" s="241"/>
+      <c r="I14" s="242"/>
+      <c r="J14" s="243"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="206"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="206"/>
-      <c r="F16" s="206"/>
-      <c r="G16" s="206"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="206"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="206"/>
-      <c r="F17" s="206"/>
-      <c r="G17" s="206"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="193"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="193"/>
+      <c r="J18" s="193"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="206"/>
-      <c r="F19" s="206"/>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="193"/>
+      <c r="G22" s="193"/>
+      <c r="H22" s="193"/>
+      <c r="I22" s="193"/>
+      <c r="J22" s="193"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="206"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
+      <c r="E23" s="193"/>
+      <c r="F23" s="193"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+      <c r="J23" s="193"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="206"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="193"/>
+      <c r="G24" s="193"/>
+      <c r="H24" s="193"/>
+      <c r="I24" s="193"/>
+      <c r="J24" s="193"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
+      <c r="E25" s="193"/>
+      <c r="F25" s="193"/>
+      <c r="G25" s="193"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="193"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="206"/>
-      <c r="F26" s="206"/>
-      <c r="G26" s="206"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="206"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="G26" s="193"/>
+      <c r="H26" s="193"/>
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="206"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="206"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="193"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="193"/>
+      <c r="J27" s="193"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="206"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="206"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="193"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="206"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="206"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="206"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="193"/>
+      <c r="G29" s="193"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="193"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="206"/>
-      <c r="F30" s="206"/>
-      <c r="G30" s="206"/>
-      <c r="H30" s="206"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="206"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="206"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="206"/>
-      <c r="F32" s="206"/>
-      <c r="G32" s="206"/>
-      <c r="H32" s="206"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="206"/>
+      <c r="E32" s="193"/>
+      <c r="F32" s="193"/>
+      <c r="G32" s="193"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="206"/>
-      <c r="F33" s="206"/>
-      <c r="G33" s="206"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="206"/>
+      <c r="E33" s="193"/>
+      <c r="F33" s="193"/>
+      <c r="G33" s="193"/>
+      <c r="H33" s="193"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="193"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="206"/>
-      <c r="F34" s="206"/>
-      <c r="G34" s="206"/>
-      <c r="H34" s="206"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="206"/>
+      <c r="E34" s="193"/>
+      <c r="F34" s="193"/>
+      <c r="G34" s="193"/>
+      <c r="H34" s="193"/>
+      <c r="I34" s="193"/>
+      <c r="J34" s="193"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="206"/>
-      <c r="F35" s="206"/>
-      <c r="G35" s="206"/>
-      <c r="H35" s="206"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="206"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="193"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="193"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="206"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="206"/>
-      <c r="F37" s="206"/>
-      <c r="G37" s="206"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="206"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="206"/>
-      <c r="F38" s="206"/>
-      <c r="G38" s="206"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="206"/>
+      <c r="E38" s="193"/>
+      <c r="F38" s="193"/>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="193"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="206"/>
-      <c r="F39" s="206"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="206"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="206"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="193"/>
+      <c r="H39" s="193"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="206"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="206"/>
-      <c r="F41" s="206"/>
-      <c r="G41" s="206"/>
-      <c r="H41" s="206"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="206"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="193"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="193"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="206"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="206"/>
-      <c r="H42" s="206"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="206"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="193"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
@@ -8342,6 +8472,30 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -8377,10 +8531,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -8405,14 +8559,14 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -8439,20 +8593,20 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="250"/>
-      <c r="B3" s="251"/>
-      <c r="C3" s="251"/>
-      <c r="D3" s="251"/>
-      <c r="E3" s="251"/>
-      <c r="F3" s="251"/>
-      <c r="G3" s="251"/>
-      <c r="H3" s="251"/>
-      <c r="I3" s="251"/>
-      <c r="J3" s="252"/>
+      <c r="A3" s="249"/>
+      <c r="B3" s="250"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="250"/>
+      <c r="E3" s="250"/>
+      <c r="F3" s="250"/>
+      <c r="G3" s="250"/>
+      <c r="H3" s="250"/>
+      <c r="I3" s="250"/>
+      <c r="J3" s="251"/>
     </row>
     <row r="4" spans="1:10" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
@@ -8467,16 +8621,16 @@
       <c r="D4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="246" t="s">
+      <c r="E4" s="245" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="246"/>
-      <c r="G4" s="247" t="s">
+      <c r="F4" s="245"/>
+      <c r="G4" s="246" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="248"/>
-      <c r="I4" s="248"/>
-      <c r="J4" s="249"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="248"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -8603,347 +8757,351 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="206"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="206"/>
-      <c r="F16" s="206"/>
-      <c r="G16" s="206"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="206"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="206"/>
-      <c r="F17" s="206"/>
-      <c r="G17" s="206"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="193"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="193"/>
+      <c r="J18" s="193"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="206"/>
-      <c r="F19" s="206"/>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="193"/>
+      <c r="G22" s="193"/>
+      <c r="H22" s="193"/>
+      <c r="I22" s="193"/>
+      <c r="J22" s="193"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="206"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
+      <c r="E23" s="193"/>
+      <c r="F23" s="193"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+      <c r="J23" s="193"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="206"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="193"/>
+      <c r="G24" s="193"/>
+      <c r="H24" s="193"/>
+      <c r="I24" s="193"/>
+      <c r="J24" s="193"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
+      <c r="E25" s="193"/>
+      <c r="F25" s="193"/>
+      <c r="G25" s="193"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="193"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="206"/>
-      <c r="F26" s="206"/>
-      <c r="G26" s="206"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="206"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="G26" s="193"/>
+      <c r="H26" s="193"/>
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="206"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="206"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="193"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="193"/>
+      <c r="J27" s="193"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="206"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="206"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="193"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="206"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="206"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="206"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="193"/>
+      <c r="G29" s="193"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="193"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="206"/>
-      <c r="F30" s="206"/>
-      <c r="G30" s="206"/>
-      <c r="H30" s="206"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="206"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="206"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="206"/>
-      <c r="F32" s="206"/>
-      <c r="G32" s="206"/>
-      <c r="H32" s="206"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="206"/>
+      <c r="E32" s="193"/>
+      <c r="F32" s="193"/>
+      <c r="G32" s="193"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="206"/>
-      <c r="F33" s="206"/>
-      <c r="G33" s="206"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="206"/>
+      <c r="E33" s="193"/>
+      <c r="F33" s="193"/>
+      <c r="G33" s="193"/>
+      <c r="H33" s="193"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="193"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="206"/>
-      <c r="F34" s="206"/>
-      <c r="G34" s="206"/>
-      <c r="H34" s="206"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="206"/>
+      <c r="E34" s="193"/>
+      <c r="F34" s="193"/>
+      <c r="G34" s="193"/>
+      <c r="H34" s="193"/>
+      <c r="I34" s="193"/>
+      <c r="J34" s="193"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="206"/>
-      <c r="F35" s="206"/>
-      <c r="G35" s="206"/>
-      <c r="H35" s="206"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="206"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="193"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="193"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="206"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="206"/>
-      <c r="F37" s="206"/>
-      <c r="G37" s="206"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="206"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="206"/>
-      <c r="F38" s="206"/>
-      <c r="G38" s="206"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="206"/>
+      <c r="E38" s="193"/>
+      <c r="F38" s="193"/>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="193"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="206"/>
-      <c r="F39" s="206"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="206"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="206"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="193"/>
+      <c r="H39" s="193"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="206"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="206"/>
-      <c r="F41" s="206"/>
-      <c r="G41" s="206"/>
-      <c r="H41" s="206"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="206"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="193"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="193"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="206"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="206"/>
-      <c r="H42" s="206"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="206"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="193"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E24:J24"/>
     <mergeCell ref="E41:J41"/>
     <mergeCell ref="E42:J42"/>
     <mergeCell ref="E31:J31"/>
@@ -8956,18 +9114,14 @@
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="E39:J39"/>
     <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -8984,8 +9138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:L7"/>
+    <sheetView view="pageBreakPreview" topLeftCell="J7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9011,10 +9165,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9039,9 +9193,9 @@
       <c r="I1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="126">
+      <c r="J1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
@@ -9052,8 +9206,8 @@
       <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9080,7 +9234,7 @@
       </c>
       <c r="J2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -9091,16 +9245,16 @@
       <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="250"/>
-      <c r="B3" s="251"/>
-      <c r="C3" s="251"/>
-      <c r="D3" s="251"/>
-      <c r="E3" s="251"/>
-      <c r="F3" s="251"/>
-      <c r="G3" s="251"/>
-      <c r="H3" s="251"/>
-      <c r="I3" s="251"/>
-      <c r="J3" s="252"/>
+      <c r="A3" s="249"/>
+      <c r="B3" s="250"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="250"/>
+      <c r="E3" s="250"/>
+      <c r="F3" s="250"/>
+      <c r="G3" s="250"/>
+      <c r="H3" s="250"/>
+      <c r="I3" s="250"/>
+      <c r="J3" s="251"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -9134,12 +9288,12 @@
       <c r="H4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="247" t="s">
+      <c r="I4" s="246" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="248"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="249"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
+      <c r="L4" s="248"/>
       <c r="M4" s="66" t="s">
         <v>44</v>
       </c>
@@ -9173,12 +9327,12 @@
       <c r="H5" s="164" t="s">
         <v>223</v>
       </c>
-      <c r="I5" s="253" t="s">
+      <c r="I5" s="252" t="s">
         <v>224</v>
       </c>
-      <c r="J5" s="254"/>
-      <c r="K5" s="254"/>
-      <c r="L5" s="255"/>
+      <c r="J5" s="253"/>
+      <c r="K5" s="253"/>
+      <c r="L5" s="254"/>
       <c r="M5" s="164"/>
       <c r="N5" s="163"/>
       <c r="O5" s="168" t="s">
@@ -9206,12 +9360,12 @@
       <c r="H6" s="164" t="s">
         <v>227</v>
       </c>
-      <c r="I6" s="256" t="s">
+      <c r="I6" s="255" t="s">
         <v>228</v>
       </c>
-      <c r="J6" s="257"/>
-      <c r="K6" s="257"/>
-      <c r="L6" s="258"/>
+      <c r="J6" s="256"/>
+      <c r="K6" s="256"/>
+      <c r="L6" s="257"/>
       <c r="M6" s="185" t="s">
         <v>230</v>
       </c>
@@ -9239,12 +9393,12 @@
       <c r="H7" s="164" t="s">
         <v>233</v>
       </c>
-      <c r="I7" s="256" t="s">
+      <c r="I7" s="255" t="s">
         <v>249</v>
       </c>
-      <c r="J7" s="257"/>
-      <c r="K7" s="257"/>
-      <c r="L7" s="258"/>
+      <c r="J7" s="256"/>
+      <c r="K7" s="256"/>
+      <c r="L7" s="257"/>
       <c r="M7" s="189" t="s">
         <v>234</v>
       </c>
@@ -9272,36 +9426,58 @@
       <c r="H8" s="164" t="s">
         <v>239</v>
       </c>
-      <c r="I8" s="253" t="s">
+      <c r="I8" s="252" t="s">
         <v>245</v>
       </c>
-      <c r="J8" s="254"/>
-      <c r="K8" s="254"/>
-      <c r="L8" s="255"/>
+      <c r="J8" s="253"/>
+      <c r="K8" s="253"/>
+      <c r="L8" s="254"/>
       <c r="M8" s="157"/>
       <c r="N8" s="157"/>
       <c r="O8" s="157"/>
       <c r="P8" s="157"/>
       <c r="Q8" s="157"/>
     </row>
-    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="242"/>
-      <c r="J9" s="243"/>
-      <c r="K9" s="243"/>
-      <c r="L9" s="244"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
+    <row r="9" spans="1:17" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="273"/>
+      <c r="B9" s="265" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="274"/>
+      <c r="D9" s="264"/>
+      <c r="E9" s="269" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="275" t="s">
+        <v>221</v>
+      </c>
+      <c r="G9" s="275" t="s">
+        <v>258</v>
+      </c>
+      <c r="H9" s="268" t="s">
+        <v>264</v>
+      </c>
+      <c r="I9" s="270" t="s">
+        <v>259</v>
+      </c>
+      <c r="J9" s="271"/>
+      <c r="K9" s="271"/>
+      <c r="L9" s="272"/>
+      <c r="M9" s="276" t="s">
+        <v>260</v>
+      </c>
+      <c r="N9" s="268" t="s">
+        <v>261</v>
+      </c>
+      <c r="O9" s="277" t="s">
+        <v>262</v>
+      </c>
+      <c r="P9" s="277" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q9" s="269" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
@@ -9312,10 +9488,10 @@
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
-      <c r="I10" s="242"/>
-      <c r="J10" s="243"/>
-      <c r="K10" s="243"/>
-      <c r="L10" s="244"/>
+      <c r="I10" s="241"/>
+      <c r="J10" s="242"/>
+      <c r="K10" s="242"/>
+      <c r="L10" s="243"/>
       <c r="M10" s="60"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
@@ -9331,10 +9507,10 @@
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
       <c r="H11" s="51"/>
-      <c r="I11" s="242"/>
-      <c r="J11" s="243"/>
-      <c r="K11" s="243"/>
-      <c r="L11" s="244"/>
+      <c r="I11" s="241"/>
+      <c r="J11" s="242"/>
+      <c r="K11" s="242"/>
+      <c r="L11" s="243"/>
       <c r="M11" s="60"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
@@ -9350,10 +9526,10 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
       <c r="H12" s="51"/>
-      <c r="I12" s="242"/>
-      <c r="J12" s="243"/>
-      <c r="K12" s="243"/>
-      <c r="L12" s="244"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="242"/>
+      <c r="K12" s="242"/>
+      <c r="L12" s="243"/>
       <c r="M12" s="60"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
@@ -9369,10 +9545,10 @@
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
-      <c r="I13" s="242"/>
-      <c r="J13" s="243"/>
-      <c r="K13" s="243"/>
-      <c r="L13" s="244"/>
+      <c r="I13" s="241"/>
+      <c r="J13" s="242"/>
+      <c r="K13" s="242"/>
+      <c r="L13" s="243"/>
       <c r="M13" s="60"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
@@ -9388,10 +9564,10 @@
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
       <c r="H14" s="55"/>
-      <c r="I14" s="242"/>
-      <c r="J14" s="243"/>
-      <c r="K14" s="243"/>
-      <c r="L14" s="244"/>
+      <c r="I14" s="241"/>
+      <c r="J14" s="242"/>
+      <c r="K14" s="242"/>
+      <c r="L14" s="243"/>
       <c r="M14" s="60"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
@@ -9403,364 +9579,339 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="206"/>
-      <c r="J15" s="206"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="206"/>
-      <c r="F16" s="206"/>
-      <c r="G16" s="206"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="206"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="206"/>
-      <c r="F17" s="206"/>
-      <c r="G17" s="206"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
+      <c r="E18" s="193"/>
+      <c r="F18" s="193"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="193"/>
+      <c r="J18" s="193"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="206"/>
-      <c r="F19" s="206"/>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="206"/>
-      <c r="F20" s="206"/>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="193"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="193"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="206"/>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="193"/>
+      <c r="G22" s="193"/>
+      <c r="H22" s="193"/>
+      <c r="I22" s="193"/>
+      <c r="J22" s="193"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="206"/>
-      <c r="F23" s="206"/>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
+      <c r="E23" s="193"/>
+      <c r="F23" s="193"/>
+      <c r="G23" s="193"/>
+      <c r="H23" s="193"/>
+      <c r="I23" s="193"/>
+      <c r="J23" s="193"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="206"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="193"/>
+      <c r="G24" s="193"/>
+      <c r="H24" s="193"/>
+      <c r="I24" s="193"/>
+      <c r="J24" s="193"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
+      <c r="E25" s="193"/>
+      <c r="F25" s="193"/>
+      <c r="G25" s="193"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="193"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="206"/>
-      <c r="F26" s="206"/>
-      <c r="G26" s="206"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="206"/>
-      <c r="J26" s="206"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="193"/>
+      <c r="G26" s="193"/>
+      <c r="H26" s="193"/>
+      <c r="I26" s="193"/>
+      <c r="J26" s="193"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="206"/>
-      <c r="I27" s="206"/>
-      <c r="J27" s="206"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="193"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="193"/>
+      <c r="J27" s="193"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="206"/>
-      <c r="I28" s="206"/>
-      <c r="J28" s="206"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="193"/>
+      <c r="H28" s="193"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="193"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="206"/>
-      <c r="F29" s="206"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="206"/>
-      <c r="I29" s="206"/>
-      <c r="J29" s="206"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="193"/>
+      <c r="G29" s="193"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="193"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="206"/>
-      <c r="F30" s="206"/>
-      <c r="G30" s="206"/>
-      <c r="H30" s="206"/>
-      <c r="I30" s="206"/>
-      <c r="J30" s="206"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="193"/>
+      <c r="H30" s="193"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="206"/>
-      <c r="F31" s="206"/>
-      <c r="G31" s="206"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="206"/>
-      <c r="J31" s="206"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="206"/>
-      <c r="F32" s="206"/>
-      <c r="G32" s="206"/>
-      <c r="H32" s="206"/>
-      <c r="I32" s="206"/>
-      <c r="J32" s="206"/>
+      <c r="E32" s="193"/>
+      <c r="F32" s="193"/>
+      <c r="G32" s="193"/>
+      <c r="H32" s="193"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="206"/>
-      <c r="F33" s="206"/>
-      <c r="G33" s="206"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="206"/>
-      <c r="J33" s="206"/>
+      <c r="E33" s="193"/>
+      <c r="F33" s="193"/>
+      <c r="G33" s="193"/>
+      <c r="H33" s="193"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="193"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="206"/>
-      <c r="F34" s="206"/>
-      <c r="G34" s="206"/>
-      <c r="H34" s="206"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="206"/>
+      <c r="E34" s="193"/>
+      <c r="F34" s="193"/>
+      <c r="G34" s="193"/>
+      <c r="H34" s="193"/>
+      <c r="I34" s="193"/>
+      <c r="J34" s="193"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="206"/>
-      <c r="F35" s="206"/>
-      <c r="G35" s="206"/>
-      <c r="H35" s="206"/>
-      <c r="I35" s="206"/>
-      <c r="J35" s="206"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="193"/>
+      <c r="H35" s="193"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="193"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="206"/>
-      <c r="F36" s="206"/>
-      <c r="G36" s="206"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="206"/>
-      <c r="J36" s="206"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="206"/>
-      <c r="F37" s="206"/>
-      <c r="G37" s="206"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="206"/>
-      <c r="J37" s="206"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="206"/>
-      <c r="F38" s="206"/>
-      <c r="G38" s="206"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="206"/>
-      <c r="J38" s="206"/>
+      <c r="E38" s="193"/>
+      <c r="F38" s="193"/>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="193"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="206"/>
-      <c r="F39" s="206"/>
-      <c r="G39" s="206"/>
-      <c r="H39" s="206"/>
-      <c r="I39" s="206"/>
-      <c r="J39" s="206"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="193"/>
+      <c r="G39" s="193"/>
+      <c r="H39" s="193"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="193"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="206"/>
-      <c r="F40" s="206"/>
-      <c r="G40" s="206"/>
-      <c r="H40" s="206"/>
-      <c r="I40" s="206"/>
-      <c r="J40" s="206"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="206"/>
-      <c r="F41" s="206"/>
-      <c r="G41" s="206"/>
-      <c r="H41" s="206"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="206"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="193"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="193"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="206"/>
-      <c r="F42" s="206"/>
-      <c r="G42" s="206"/>
-      <c r="H42" s="206"/>
-      <c r="I42" s="206"/>
-      <c r="J42" s="206"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="193"/>
+      <c r="H42" s="193"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
     <mergeCell ref="E42:J42"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="I5:L5"/>
@@ -9777,6 +9928,31 @@
     <mergeCell ref="E29:J29"/>
     <mergeCell ref="E30:J30"/>
     <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2">
@@ -9785,10 +9961,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5">
       <formula1>"Load,Click,Double Click,Change,Selected,KeyDown,KeyPress,Hover,Focus,LostFocus"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G9">
       <formula1>"SQL Script, ID SQL, ID Store, ID Function, ID Trigger"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F9">
       <formula1>"Select,Insert,Update,Delete"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5"/>
@@ -9803,8 +9979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9823,11 +9999,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9852,15 +10028,15 @@
       <c r="J1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="126">
+      <c r="K1" s="126" t="str">
         <f>'Update History'!J1</f>
-        <v>0</v>
+        <v>Thị Phượng</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9887,7 +10063,7 @@
       </c>
       <c r="K2" s="15">
         <f>'Update History'!J2</f>
-        <v>0</v>
+        <v>42381</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10200,19 +10376,22 @@
       <c r="J23" s="169"/>
       <c r="K23" s="170"/>
     </row>
-    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="174"/>
-      <c r="B24" s="173"/>
-      <c r="C24" s="182"/>
-      <c r="D24" s="172"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="177"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="17"/>
+    <row r="24" spans="1:12" s="281" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="278" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24" s="278"/>
+      <c r="C24" s="279" t="s">
+        <v>267</v>
+      </c>
+      <c r="D24" s="279"/>
+      <c r="E24" s="279"/>
+      <c r="F24" s="279"/>
+      <c r="G24" s="279"/>
+      <c r="H24" s="279"/>
+      <c r="I24" s="279"/>
+      <c r="J24" s="279"/>
+      <c r="K24" s="280"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="171" t="s">
@@ -10296,12 +10475,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="259"/>
-      <c r="G30" s="259"/>
-      <c r="H30" s="259"/>
-      <c r="I30" s="259"/>
-      <c r="J30" s="259"/>
-      <c r="K30" s="259"/>
+      <c r="F30" s="258"/>
+      <c r="G30" s="258"/>
+      <c r="H30" s="258"/>
+      <c r="I30" s="258"/>
+      <c r="J30" s="258"/>
+      <c r="K30" s="258"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10310,12 +10489,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="259"/>
-      <c r="G31" s="259"/>
-      <c r="H31" s="259"/>
-      <c r="I31" s="259"/>
-      <c r="J31" s="259"/>
-      <c r="K31" s="259"/>
+      <c r="F31" s="258"/>
+      <c r="G31" s="258"/>
+      <c r="H31" s="258"/>
+      <c r="I31" s="258"/>
+      <c r="J31" s="258"/>
+      <c r="K31" s="258"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10324,12 +10503,12 @@
       <c r="C32" s="39"/>
       <c r="D32" s="42"/>
       <c r="E32" s="38"/>
-      <c r="F32" s="259"/>
-      <c r="G32" s="259"/>
-      <c r="H32" s="259"/>
-      <c r="I32" s="259"/>
-      <c r="J32" s="259"/>
-      <c r="K32" s="259"/>
+      <c r="F32" s="258"/>
+      <c r="G32" s="258"/>
+      <c r="H32" s="258"/>
+      <c r="I32" s="258"/>
+      <c r="J32" s="258"/>
+      <c r="K32" s="258"/>
       <c r="L32" s="17"/>
     </row>
     <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10338,12 +10517,12 @@
       <c r="C33" s="39"/>
       <c r="D33" s="42"/>
       <c r="E33" s="38"/>
-      <c r="F33" s="259"/>
-      <c r="G33" s="259"/>
-      <c r="H33" s="259"/>
-      <c r="I33" s="259"/>
-      <c r="J33" s="259"/>
-      <c r="K33" s="259"/>
+      <c r="F33" s="258"/>
+      <c r="G33" s="258"/>
+      <c r="H33" s="258"/>
+      <c r="I33" s="258"/>
+      <c r="J33" s="258"/>
+      <c r="K33" s="258"/>
       <c r="L33" s="17"/>
     </row>
     <row r="34" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -10529,12 +10708,13 @@
       <c r="L46" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="F30:K30"/>
     <mergeCell ref="F31:K31"/>
     <mergeCell ref="F32:K32"/>
     <mergeCell ref="F33:K33"/>
     <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C24:K24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -10571,11 +10751,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -10598,9 +10778,9 @@
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196"/>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -10970,12 +11150,12 @@
       <c r="C28" s="39"/>
       <c r="D28" s="42"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="259"/>
-      <c r="G28" s="259"/>
-      <c r="H28" s="259"/>
-      <c r="I28" s="259"/>
-      <c r="J28" s="259"/>
-      <c r="K28" s="259"/>
+      <c r="F28" s="258"/>
+      <c r="G28" s="258"/>
+      <c r="H28" s="258"/>
+      <c r="I28" s="258"/>
+      <c r="J28" s="258"/>
+      <c r="K28" s="258"/>
       <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10984,12 +11164,12 @@
       <c r="C29" s="39"/>
       <c r="D29" s="42"/>
       <c r="E29" s="38"/>
-      <c r="F29" s="259"/>
-      <c r="G29" s="259"/>
-      <c r="H29" s="259"/>
-      <c r="I29" s="259"/>
-      <c r="J29" s="259"/>
-      <c r="K29" s="259"/>
+      <c r="F29" s="258"/>
+      <c r="G29" s="258"/>
+      <c r="H29" s="258"/>
+      <c r="I29" s="258"/>
+      <c r="J29" s="258"/>
+      <c r="K29" s="258"/>
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -10998,12 +11178,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="259"/>
-      <c r="G30" s="259"/>
-      <c r="H30" s="259"/>
-      <c r="I30" s="259"/>
-      <c r="J30" s="259"/>
-      <c r="K30" s="259"/>
+      <c r="F30" s="258"/>
+      <c r="G30" s="258"/>
+      <c r="H30" s="258"/>
+      <c r="I30" s="258"/>
+      <c r="J30" s="258"/>
+      <c r="K30" s="258"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11012,12 +11192,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="259"/>
-      <c r="G31" s="259"/>
-      <c r="H31" s="259"/>
-      <c r="I31" s="259"/>
-      <c r="J31" s="259"/>
-      <c r="K31" s="259"/>
+      <c r="F31" s="258"/>
+      <c r="G31" s="258"/>
+      <c r="H31" s="258"/>
+      <c r="I31" s="258"/>
+      <c r="J31" s="258"/>
+      <c r="K31" s="258"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -11237,14 +11417,14 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="E2" s="260" t="s">
+      <c r="E2" s="259" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
-      <c r="J2" s="260"/>
+      <c r="F2" s="259"/>
+      <c r="G2" s="259"/>
+      <c r="H2" s="259"/>
+      <c r="I2" s="259"/>
+      <c r="J2" s="259"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
@@ -11665,11 +11845,11 @@
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
       <c r="D28" s="78"/>
-      <c r="E28" s="261" t="s">
+      <c r="E28" s="260" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="262"/>
-      <c r="G28" s="263"/>
+      <c r="F28" s="261"/>
+      <c r="G28" s="262"/>
       <c r="H28" s="78"/>
       <c r="I28" s="78"/>
       <c r="J28" s="78"/>

</xml_diff>